<commit_message>
Add shopped and planned dates fields
</commit_message>
<xml_diff>
--- a/groceries.xlsx
+++ b/groceries.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Groceries" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,9 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
-  <si>
-    <t xml:space="preserve">date</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+  <si>
+    <t xml:space="preserve">planned</t>
   </si>
   <si>
     <t xml:space="preserve">price</t>
@@ -50,13 +50,16 @@
     <t xml:space="preserve">who</t>
   </si>
   <si>
+    <t xml:space="preserve">shopped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total</t>
+  </si>
+  <si>
     <t xml:space="preserve">where</t>
   </si>
   <si>
     <t xml:space="preserve">what</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total</t>
   </si>
   <si>
     <t xml:space="preserve">tax</t>
@@ -493,12 +496,12 @@
   </sheetPr>
   <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -556,8 +559,8 @@
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
+      <c r="B2" s="4" t="n">
+        <v>45292</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="10" t="n">
@@ -569,7 +572,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I2" s="11" t="n">
         <f aca="false">SUM(I4:I103)</f>
@@ -581,22 +584,26 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="29.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -3441,15 +3448,13 @@
     </row>
   </sheetData>
   <autoFilter ref="A3:K33"/>
-  <mergeCells count="8">
+  <mergeCells count="6">
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="J1:J3"/>
     <mergeCell ref="K1:K3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="I2">
     <cfRule type="cellIs" priority="2" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
@@ -3480,7 +3485,7 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3488,130 +3493,130 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B12" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>